<commit_message>
finalized version for order placement
</commit_message>
<xml_diff>
--- a/RFSoC_directclocking/pinPlanning.xlsx
+++ b/RFSoC_directclocking/pinPlanning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\codya\repo\rfsoc-interface\RFSoC_directclocking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{B033FCBA-1C4B-4DF5-9174-0F445B2AC041}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96244EA3-2D89-4641-BC20-445B1FB925C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="29829" windowHeight="18120" xr2:uid="{2A5425FC-9E25-44BF-8057-789C819589DB}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="19">
   <si>
     <t>NC</t>
   </si>
@@ -55,9 +55,6 @@
     <t>EXPOSED PAD GND</t>
   </si>
   <si>
-    <t>Unconnected</t>
-  </si>
-  <si>
     <t>Bidirectional</t>
   </si>
   <si>
@@ -94,13 +91,7 @@
     <t>Left</t>
   </si>
   <si>
-    <t>Right</t>
-  </si>
-  <si>
-    <t>Up</t>
-  </si>
-  <si>
-    <t>Down</t>
+    <t>Passive</t>
   </si>
 </sst>
 </file>
@@ -148,7 +139,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -171,16 +162,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -503,7 +506,7 @@
   <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:I33"/>
+      <selection activeCell="G2" sqref="G2:G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -513,30 +516,30 @@
     <col min="4" max="4" width="13.07421875" customWidth="1"/>
     <col min="5" max="5" width="14.3046875" customWidth="1"/>
     <col min="6" max="6" width="11.3828125" customWidth="1"/>
-    <col min="7" max="7" width="13.3046875" customWidth="1"/>
+    <col min="7" max="7" width="12.53515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>12</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>13</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>14</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>15</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>16</v>
-      </c>
-      <c r="G1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.4">
@@ -547,27 +550,27 @@
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F2" s="1">
-        <v>1.7</v>
-      </c>
-      <c r="G2" s="1">
-        <v>0</v>
-      </c>
-      <c r="H2" t="str">
-        <f>F2&amp;" in"</f>
-        <v>1.7 in</v>
-      </c>
-      <c r="I2" t="str">
-        <f>G2&amp;" in"</f>
-        <v>0 in</v>
+        <v>17</v>
+      </c>
+      <c r="F2" t="str">
+        <f>H2&amp;" in"</f>
+        <v>1.45 in</v>
+      </c>
+      <c r="G2" t="str">
+        <f>I2&amp;" in"</f>
+        <v>-2 in</v>
+      </c>
+      <c r="H2" s="1">
+        <v>1.45</v>
+      </c>
+      <c r="I2" s="1">
+        <v>-2</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.4">
@@ -578,27 +581,27 @@
         <v>0</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F3" s="1">
-        <v>1.5</v>
-      </c>
-      <c r="G3" s="1">
-        <v>0</v>
-      </c>
-      <c r="H3" t="str">
-        <f t="shared" ref="H3:H33" si="0">F3&amp;" in"</f>
-        <v>1.5 in</v>
-      </c>
-      <c r="I3" t="str">
-        <f t="shared" ref="I3:I33" si="1">G3&amp;" in"</f>
-        <v>0 in</v>
+        <v>17</v>
+      </c>
+      <c r="F3" t="str">
+        <f>H3&amp;" in"</f>
+        <v>1.45 in</v>
+      </c>
+      <c r="G3" t="str">
+        <f>I3&amp;" in"</f>
+        <v>-2 in</v>
+      </c>
+      <c r="H3" s="1">
+        <v>1.45</v>
+      </c>
+      <c r="I3" s="1">
+        <v>-2</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.4">
@@ -609,27 +612,27 @@
         <v>0</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" s="1">
-        <v>1.3</v>
-      </c>
-      <c r="G4" s="1">
-        <v>0</v>
-      </c>
-      <c r="H4" t="str">
-        <f t="shared" si="0"/>
-        <v>1.3 in</v>
-      </c>
-      <c r="I4" t="str">
-        <f t="shared" si="1"/>
-        <v>0 in</v>
+        <v>17</v>
+      </c>
+      <c r="F4" t="str">
+        <f>H4&amp;" in"</f>
+        <v>1.45 in</v>
+      </c>
+      <c r="G4" t="str">
+        <f>I4&amp;" in"</f>
+        <v>-2 in</v>
+      </c>
+      <c r="H4" s="1">
+        <v>1.45</v>
+      </c>
+      <c r="I4" s="1">
+        <v>-2</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.4">
@@ -640,27 +643,27 @@
         <v>0</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" s="1">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="G5" s="1">
-        <v>0</v>
-      </c>
-      <c r="H5" t="str">
-        <f t="shared" si="0"/>
-        <v>1.1 in</v>
-      </c>
-      <c r="I5" t="str">
-        <f t="shared" si="1"/>
-        <v>0 in</v>
+        <v>17</v>
+      </c>
+      <c r="F5" t="str">
+        <f>H5&amp;" in"</f>
+        <v>1.45 in</v>
+      </c>
+      <c r="G5" t="str">
+        <f>I5&amp;" in"</f>
+        <v>-2 in</v>
+      </c>
+      <c r="H5" s="1">
+        <v>1.45</v>
+      </c>
+      <c r="I5" s="1">
+        <v>-2</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.4">
@@ -671,27 +674,27 @@
         <v>0</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" s="1">
-        <v>0.9</v>
-      </c>
-      <c r="G6" s="1">
-        <v>0</v>
-      </c>
-      <c r="H6" t="str">
-        <f t="shared" si="0"/>
-        <v>0.9 in</v>
-      </c>
-      <c r="I6" t="str">
-        <f t="shared" si="1"/>
-        <v>0 in</v>
+        <v>17</v>
+      </c>
+      <c r="F6" t="str">
+        <f>H6&amp;" in"</f>
+        <v>1.45 in</v>
+      </c>
+      <c r="G6" t="str">
+        <f>I6&amp;" in"</f>
+        <v>-2 in</v>
+      </c>
+      <c r="H6" s="1">
+        <v>1.45</v>
+      </c>
+      <c r="I6" s="1">
+        <v>-2</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.4">
@@ -702,27 +705,27 @@
         <v>0</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F7" s="1">
-        <v>0.7</v>
-      </c>
-      <c r="G7" s="1">
-        <v>0</v>
-      </c>
-      <c r="H7" t="str">
-        <f t="shared" si="0"/>
-        <v>0.7 in</v>
-      </c>
-      <c r="I7" t="str">
-        <f t="shared" si="1"/>
-        <v>0 in</v>
+        <v>17</v>
+      </c>
+      <c r="F7" t="str">
+        <f>H7&amp;" in"</f>
+        <v>1.45 in</v>
+      </c>
+      <c r="G7" t="str">
+        <f>I7&amp;" in"</f>
+        <v>-2 in</v>
+      </c>
+      <c r="H7" s="1">
+        <v>1.45</v>
+      </c>
+      <c r="I7" s="1">
+        <v>-2</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.4">
@@ -733,27 +736,27 @@
         <v>0</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F8" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="G8" s="1">
-        <v>0</v>
-      </c>
-      <c r="H8" t="str">
-        <f t="shared" si="0"/>
-        <v>0.5 in</v>
-      </c>
-      <c r="I8" t="str">
-        <f t="shared" si="1"/>
-        <v>0 in</v>
+        <v>17</v>
+      </c>
+      <c r="F8" t="str">
+        <f>H8&amp;" in"</f>
+        <v>1.45 in</v>
+      </c>
+      <c r="G8" t="str">
+        <f>I8&amp;" in"</f>
+        <v>-2 in</v>
+      </c>
+      <c r="H8" s="1">
+        <v>1.45</v>
+      </c>
+      <c r="I8" s="1">
+        <v>-2</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.4">
@@ -764,27 +767,27 @@
         <v>0</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F9" s="1">
-        <v>0.3</v>
-      </c>
-      <c r="G9" s="1">
-        <v>0</v>
-      </c>
-      <c r="H9" t="str">
-        <f t="shared" si="0"/>
-        <v>0.3 in</v>
-      </c>
-      <c r="I9" t="str">
-        <f t="shared" si="1"/>
-        <v>0 in</v>
+        <v>17</v>
+      </c>
+      <c r="F9" t="str">
+        <f>H9&amp;" in"</f>
+        <v>1.45 in</v>
+      </c>
+      <c r="G9" t="str">
+        <f>I9&amp;" in"</f>
+        <v>-2 in</v>
+      </c>
+      <c r="H9" s="1">
+        <v>1.45</v>
+      </c>
+      <c r="I9" s="1">
+        <v>-2</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.4">
@@ -795,27 +798,27 @@
         <v>1</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F10" s="2">
-        <v>0</v>
-      </c>
-      <c r="G10" s="2">
-        <v>-0.3</v>
-      </c>
-      <c r="H10" t="str">
-        <f t="shared" si="0"/>
-        <v>0 in</v>
-      </c>
-      <c r="I10" t="str">
-        <f t="shared" si="1"/>
-        <v>-0.3 in</v>
+        <v>9</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" t="str">
+        <f>H10&amp;" in"</f>
+        <v>1.45 in</v>
+      </c>
+      <c r="G10" t="str">
+        <f>I10&amp;" in"</f>
+        <v>-2 in</v>
+      </c>
+      <c r="H10" s="1">
+        <v>1.45</v>
+      </c>
+      <c r="I10" s="1">
+        <v>-2</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.4">
@@ -826,27 +829,27 @@
         <v>2</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F11" s="2">
-        <v>0</v>
-      </c>
-      <c r="G11" s="2">
-        <v>-0.5</v>
-      </c>
-      <c r="H11" t="str">
-        <f t="shared" si="0"/>
-        <v>0 in</v>
-      </c>
-      <c r="I11" t="str">
-        <f t="shared" si="1"/>
-        <v>-0.5 in</v>
+        <v>9</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" t="str">
+        <f>H11&amp;" in"</f>
+        <v>1.45 in</v>
+      </c>
+      <c r="G11" t="str">
+        <f>I11&amp;" in"</f>
+        <v>0.4 in</v>
+      </c>
+      <c r="H11" s="1">
+        <v>1.45</v>
+      </c>
+      <c r="I11" s="1">
+        <v>0.4</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.4">
@@ -857,27 +860,27 @@
         <v>1</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F12" s="2">
-        <v>0</v>
-      </c>
-      <c r="G12" s="2">
-        <v>-0.7</v>
-      </c>
-      <c r="H12" t="str">
-        <f t="shared" si="0"/>
-        <v>0 in</v>
-      </c>
-      <c r="I12" t="str">
-        <f t="shared" si="1"/>
-        <v>-0.7 in</v>
+        <v>9</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" t="str">
+        <f>H12&amp;" in"</f>
+        <v>1.45 in</v>
+      </c>
+      <c r="G12" t="str">
+        <f>I12&amp;" in"</f>
+        <v>-2 in</v>
+      </c>
+      <c r="H12" s="1">
+        <v>1.45</v>
+      </c>
+      <c r="I12" s="1">
+        <v>-2</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.4">
@@ -888,27 +891,27 @@
         <v>0</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F13" s="2">
-        <v>0</v>
-      </c>
-      <c r="G13" s="2">
-        <v>-0.9</v>
-      </c>
-      <c r="H13" t="str">
-        <f t="shared" si="0"/>
-        <v>0 in</v>
-      </c>
-      <c r="I13" t="str">
-        <f t="shared" si="1"/>
-        <v>-0.9 in</v>
+        <v>9</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" t="str">
+        <f>H13&amp;" in"</f>
+        <v>1.45 in</v>
+      </c>
+      <c r="G13" t="str">
+        <f>I13&amp;" in"</f>
+        <v>-2 in</v>
+      </c>
+      <c r="H13" s="1">
+        <v>1.45</v>
+      </c>
+      <c r="I13" s="1">
+        <v>-2</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.4">
@@ -919,27 +922,27 @@
         <v>0</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F14" s="2">
-        <v>0</v>
-      </c>
-      <c r="G14" s="2">
-        <v>-1.1000000000000001</v>
-      </c>
-      <c r="H14" t="str">
-        <f t="shared" si="0"/>
-        <v>0 in</v>
-      </c>
-      <c r="I14" t="str">
-        <f t="shared" si="1"/>
-        <v>-1.1 in</v>
+        <v>9</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F14" t="str">
+        <f>H14&amp;" in"</f>
+        <v>1.45 in</v>
+      </c>
+      <c r="G14" t="str">
+        <f>I14&amp;" in"</f>
+        <v>-2 in</v>
+      </c>
+      <c r="H14" s="1">
+        <v>1.45</v>
+      </c>
+      <c r="I14" s="1">
+        <v>-2</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.4">
@@ -950,27 +953,27 @@
         <v>0</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F15" s="2">
-        <v>0</v>
-      </c>
-      <c r="G15" s="2">
-        <v>-1.3</v>
-      </c>
-      <c r="H15" t="str">
-        <f t="shared" si="0"/>
-        <v>0 in</v>
-      </c>
-      <c r="I15" t="str">
-        <f t="shared" si="1"/>
-        <v>-1.3 in</v>
+        <v>9</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F15" t="str">
+        <f>H15&amp;" in"</f>
+        <v>1.45 in</v>
+      </c>
+      <c r="G15" t="str">
+        <f>I15&amp;" in"</f>
+        <v>-2 in</v>
+      </c>
+      <c r="H15" s="1">
+        <v>1.45</v>
+      </c>
+      <c r="I15" s="1">
+        <v>-2</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.4">
@@ -981,27 +984,27 @@
         <v>0</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F16" s="2">
-        <v>0</v>
-      </c>
-      <c r="G16" s="2">
-        <v>-1.5</v>
-      </c>
-      <c r="H16" t="str">
-        <f t="shared" si="0"/>
-        <v>0 in</v>
-      </c>
-      <c r="I16" t="str">
-        <f t="shared" si="1"/>
-        <v>-1.5 in</v>
+        <v>9</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F16" t="str">
+        <f>H16&amp;" in"</f>
+        <v>1.45 in</v>
+      </c>
+      <c r="G16" t="str">
+        <f>I16&amp;" in"</f>
+        <v>-2 in</v>
+      </c>
+      <c r="H16" s="1">
+        <v>1.45</v>
+      </c>
+      <c r="I16" s="1">
+        <v>-2</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.4">
@@ -1012,27 +1015,27 @@
         <v>0</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F17" s="2">
-        <v>0</v>
-      </c>
-      <c r="G17" s="2">
-        <v>-1.7</v>
-      </c>
-      <c r="H17" t="str">
-        <f t="shared" si="0"/>
-        <v>0 in</v>
-      </c>
-      <c r="I17" t="str">
-        <f t="shared" si="1"/>
-        <v>-1.7 in</v>
+        <v>9</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F17" t="str">
+        <f>H17&amp;" in"</f>
+        <v>1.45 in</v>
+      </c>
+      <c r="G17" t="str">
+        <f>I17&amp;" in"</f>
+        <v>-2 in</v>
+      </c>
+      <c r="H17" s="1">
+        <v>1.45</v>
+      </c>
+      <c r="I17" s="1">
+        <v>-2</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.4">
@@ -1043,27 +1046,27 @@
         <v>0</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F18" s="3">
-        <v>0.3</v>
-      </c>
-      <c r="G18" s="3">
-        <v>-2</v>
-      </c>
-      <c r="H18" t="str">
-        <f t="shared" si="0"/>
-        <v>0.3 in</v>
-      </c>
-      <c r="I18" t="str">
-        <f t="shared" si="1"/>
-        <v>-2 in</v>
+        <v>9</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F18" t="str">
+        <f>H18&amp;" in"</f>
+        <v>1.45 in</v>
+      </c>
+      <c r="G18" t="str">
+        <f>I18&amp;" in"</f>
+        <v>-2 in</v>
+      </c>
+      <c r="H18" s="1">
+        <v>1.45</v>
+      </c>
+      <c r="I18" s="1">
+        <v>-2</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.4">
@@ -1074,27 +1077,27 @@
         <v>0</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F19" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="G19" s="3">
-        <v>-2</v>
-      </c>
-      <c r="H19" t="str">
-        <f t="shared" si="0"/>
-        <v>0.5 in</v>
-      </c>
-      <c r="I19" t="str">
-        <f t="shared" si="1"/>
-        <v>-2 in</v>
+        <v>9</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F19" t="str">
+        <f>H19&amp;" in"</f>
+        <v>1.45 in</v>
+      </c>
+      <c r="G19" t="str">
+        <f>I19&amp;" in"</f>
+        <v>-2 in</v>
+      </c>
+      <c r="H19" s="1">
+        <v>1.45</v>
+      </c>
+      <c r="I19" s="1">
+        <v>-2</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.4">
@@ -1105,27 +1108,27 @@
         <v>0</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F20" s="3">
-        <v>0.7</v>
-      </c>
-      <c r="G20" s="3">
-        <v>-2</v>
-      </c>
-      <c r="H20" t="str">
-        <f t="shared" si="0"/>
-        <v>0.7 in</v>
-      </c>
-      <c r="I20" t="str">
-        <f t="shared" si="1"/>
-        <v>-2 in</v>
+        <v>9</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F20" t="str">
+        <f>H20&amp;" in"</f>
+        <v>1.45 in</v>
+      </c>
+      <c r="G20" t="str">
+        <f>I20&amp;" in"</f>
+        <v>-2 in</v>
+      </c>
+      <c r="H20" s="1">
+        <v>1.45</v>
+      </c>
+      <c r="I20" s="1">
+        <v>-2</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.4">
@@ -1136,27 +1139,27 @@
         <v>1</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F21" s="3">
-        <v>0.9</v>
-      </c>
-      <c r="G21" s="3">
-        <v>-2</v>
-      </c>
-      <c r="H21" t="str">
-        <f t="shared" si="0"/>
-        <v>0.9 in</v>
-      </c>
-      <c r="I21" t="str">
-        <f t="shared" si="1"/>
-        <v>-2 in</v>
+        <v>9</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F21" t="str">
+        <f>H21&amp;" in"</f>
+        <v>1.45 in</v>
+      </c>
+      <c r="G21" t="str">
+        <f>I21&amp;" in"</f>
+        <v>-2 in</v>
+      </c>
+      <c r="H21" s="1">
+        <v>1.45</v>
+      </c>
+      <c r="I21" s="1">
+        <v>-2</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.4">
@@ -1167,27 +1170,27 @@
         <v>3</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F22" s="3">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="G22" s="3">
-        <v>-2</v>
-      </c>
-      <c r="H22" t="str">
-        <f t="shared" si="0"/>
-        <v>1.1 in</v>
-      </c>
-      <c r="I22" t="str">
-        <f t="shared" si="1"/>
-        <v>-2 in</v>
+        <v>9</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F22" t="str">
+        <f>H22&amp;" in"</f>
+        <v>1.45 in</v>
+      </c>
+      <c r="G22" t="str">
+        <f>I22&amp;" in"</f>
+        <v>0.2 in</v>
+      </c>
+      <c r="H22" s="1">
+        <v>1.45</v>
+      </c>
+      <c r="I22" s="1">
+        <v>0.2</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.4">
@@ -1198,27 +1201,27 @@
         <v>1</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F23" s="3">
-        <v>1.3</v>
-      </c>
-      <c r="G23" s="3">
-        <v>-2</v>
-      </c>
-      <c r="H23" t="str">
-        <f t="shared" si="0"/>
-        <v>1.3 in</v>
-      </c>
-      <c r="I23" t="str">
-        <f t="shared" si="1"/>
-        <v>-2 in</v>
+        <v>9</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F23" t="str">
+        <f>H23&amp;" in"</f>
+        <v>1.45 in</v>
+      </c>
+      <c r="G23" t="str">
+        <f>I23&amp;" in"</f>
+        <v>-2 in</v>
+      </c>
+      <c r="H23" s="1">
+        <v>1.45</v>
+      </c>
+      <c r="I23" s="1">
+        <v>-2</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.4">
@@ -1229,27 +1232,27 @@
         <v>0</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F24" s="3">
-        <v>1.5</v>
-      </c>
-      <c r="G24" s="3">
-        <v>-2</v>
-      </c>
-      <c r="H24" t="str">
-        <f t="shared" si="0"/>
-        <v>1.5 in</v>
-      </c>
-      <c r="I24" t="str">
-        <f t="shared" si="1"/>
-        <v>-2 in</v>
+        <v>9</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F24" t="str">
+        <f>H24&amp;" in"</f>
+        <v>1.45 in</v>
+      </c>
+      <c r="G24" t="str">
+        <f>I24&amp;" in"</f>
+        <v>-2 in</v>
+      </c>
+      <c r="H24" s="1">
+        <v>1.45</v>
+      </c>
+      <c r="I24" s="1">
+        <v>-2</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.4">
@@ -1260,27 +1263,27 @@
         <v>0</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F25" s="3">
-        <v>1.7</v>
-      </c>
-      <c r="G25" s="3">
-        <v>-2</v>
-      </c>
-      <c r="H25" t="str">
-        <f t="shared" si="0"/>
-        <v>1.7 in</v>
-      </c>
-      <c r="I25" t="str">
-        <f t="shared" si="1"/>
-        <v>-2 in</v>
+        <v>9</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F25" t="str">
+        <f>H25&amp;" in"</f>
+        <v>1.45 in</v>
+      </c>
+      <c r="G25" t="str">
+        <f>I25&amp;" in"</f>
+        <v>-2 in</v>
+      </c>
+      <c r="H25" s="1">
+        <v>1.45</v>
+      </c>
+      <c r="I25" s="1">
+        <v>-2</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.4">
@@ -1291,27 +1294,27 @@
         <v>0</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F26" s="4">
-        <v>2</v>
-      </c>
-      <c r="G26" s="4">
-        <v>-1.7</v>
-      </c>
-      <c r="H26" t="str">
-        <f t="shared" si="0"/>
-        <v>2 in</v>
-      </c>
-      <c r="I26" t="str">
-        <f t="shared" si="1"/>
-        <v>-1.7 in</v>
+        <v>9</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F26" t="str">
+        <f>H26&amp;" in"</f>
+        <v>1.45 in</v>
+      </c>
+      <c r="G26" t="str">
+        <f>I26&amp;" in"</f>
+        <v>-2 in</v>
+      </c>
+      <c r="H26" s="1">
+        <v>1.45</v>
+      </c>
+      <c r="I26" s="1">
+        <v>-2</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.4">
@@ -1322,27 +1325,27 @@
         <v>0</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F27" s="4">
-        <v>2</v>
-      </c>
-      <c r="G27" s="4">
-        <v>-1.5</v>
-      </c>
-      <c r="H27" t="str">
-        <f t="shared" si="0"/>
-        <v>2 in</v>
-      </c>
-      <c r="I27" t="str">
-        <f t="shared" si="1"/>
-        <v>-1.5 in</v>
+        <v>9</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F27" t="str">
+        <f>H27&amp;" in"</f>
+        <v>1.45 in</v>
+      </c>
+      <c r="G27" t="str">
+        <f>I27&amp;" in"</f>
+        <v>-2 in</v>
+      </c>
+      <c r="H27" s="1">
+        <v>1.45</v>
+      </c>
+      <c r="I27" s="1">
+        <v>-2</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.4">
@@ -1353,27 +1356,27 @@
         <v>0</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E28" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F28" s="4">
-        <v>2</v>
-      </c>
-      <c r="G28" s="4">
-        <v>-1.3</v>
-      </c>
-      <c r="H28" t="str">
-        <f t="shared" si="0"/>
-        <v>2 in</v>
-      </c>
-      <c r="I28" t="str">
-        <f t="shared" si="1"/>
-        <v>-1.3 in</v>
+        <v>9</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F28" t="str">
+        <f>H28&amp;" in"</f>
+        <v>1.45 in</v>
+      </c>
+      <c r="G28" t="str">
+        <f>I28&amp;" in"</f>
+        <v>-2 in</v>
+      </c>
+      <c r="H28" s="1">
+        <v>1.45</v>
+      </c>
+      <c r="I28" s="1">
+        <v>-2</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.4">
@@ -1384,27 +1387,27 @@
         <v>0</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F29" s="4">
-        <v>2</v>
-      </c>
-      <c r="G29" s="4">
-        <v>-1.1000000000000001</v>
-      </c>
-      <c r="H29" t="str">
-        <f t="shared" si="0"/>
-        <v>2 in</v>
-      </c>
-      <c r="I29" t="str">
-        <f t="shared" si="1"/>
-        <v>-1.1 in</v>
+        <v>9</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F29" t="str">
+        <f>H29&amp;" in"</f>
+        <v>1.45 in</v>
+      </c>
+      <c r="G29" t="str">
+        <f>I29&amp;" in"</f>
+        <v>-2 in</v>
+      </c>
+      <c r="H29" s="1">
+        <v>1.45</v>
+      </c>
+      <c r="I29" s="1">
+        <v>-2</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.4">
@@ -1415,27 +1418,27 @@
         <v>0</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F30" s="4">
-        <v>2</v>
-      </c>
-      <c r="G30" s="4">
-        <v>-0.9</v>
-      </c>
-      <c r="H30" t="str">
-        <f t="shared" si="0"/>
-        <v>2 in</v>
-      </c>
-      <c r="I30" t="str">
-        <f t="shared" si="1"/>
-        <v>-0.9 in</v>
+        <v>9</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F30" t="str">
+        <f>H30&amp;" in"</f>
+        <v>1.45 in</v>
+      </c>
+      <c r="G30" t="str">
+        <f>I30&amp;" in"</f>
+        <v>-2 in</v>
+      </c>
+      <c r="H30" s="1">
+        <v>1.45</v>
+      </c>
+      <c r="I30" s="1">
+        <v>-2</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.4">
@@ -1446,27 +1449,27 @@
         <v>1</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E31" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F31" s="4">
-        <v>2</v>
-      </c>
-      <c r="G31" s="4">
-        <v>-0.7</v>
-      </c>
-      <c r="H31" t="str">
-        <f t="shared" si="0"/>
-        <v>2 in</v>
-      </c>
-      <c r="I31" t="str">
-        <f t="shared" si="1"/>
-        <v>-0.7 in</v>
+        <v>9</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F31" t="str">
+        <f>H31&amp;" in"</f>
+        <v>1.45 in</v>
+      </c>
+      <c r="G31" t="str">
+        <f>I31&amp;" in"</f>
+        <v>-2 in</v>
+      </c>
+      <c r="H31" s="1">
+        <v>1.45</v>
+      </c>
+      <c r="I31" s="1">
+        <v>-2</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.4">
@@ -1477,27 +1480,27 @@
         <v>4</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E32" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F32" s="4">
-        <v>2</v>
-      </c>
-      <c r="G32" s="4">
-        <v>-0.5</v>
-      </c>
-      <c r="H32" t="str">
-        <f t="shared" si="0"/>
-        <v>2 in</v>
-      </c>
-      <c r="I32" t="str">
-        <f t="shared" si="1"/>
-        <v>-0.5 in</v>
+        <v>9</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F32" t="str">
+        <f>H32&amp;" in"</f>
+        <v>1.45 in</v>
+      </c>
+      <c r="G32" t="str">
+        <f>I32&amp;" in"</f>
+        <v>0 in</v>
+      </c>
+      <c r="H32" s="1">
+        <v>1.45</v>
+      </c>
+      <c r="I32" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.4">
@@ -1508,27 +1511,27 @@
         <v>1</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E33" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F33" s="4">
-        <v>2</v>
-      </c>
-      <c r="G33" s="4">
-        <v>-0.3</v>
-      </c>
-      <c r="H33" t="str">
-        <f t="shared" si="0"/>
-        <v>2 in</v>
-      </c>
-      <c r="I33" t="str">
-        <f t="shared" si="1"/>
-        <v>-0.3 in</v>
+        <v>9</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F33" t="str">
+        <f>H33&amp;" in"</f>
+        <v>1.45 in</v>
+      </c>
+      <c r="G33" t="str">
+        <f>I33&amp;" in"</f>
+        <v>-2 in</v>
+      </c>
+      <c r="H33" s="1">
+        <v>1.45</v>
+      </c>
+      <c r="I33" s="1">
+        <v>-2</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.4">
@@ -1539,10 +1542,27 @@
         <v>5</v>
       </c>
       <c r="C34" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D34" t="s">
-        <v>10</v>
+        <v>9</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F34" t="str">
+        <f>H34&amp;" in"</f>
+        <v>1.45 in</v>
+      </c>
+      <c r="G34" t="str">
+        <f>I34&amp;" in"</f>
+        <v>0.6 in</v>
+      </c>
+      <c r="H34" s="5">
+        <v>1.45</v>
+      </c>
+      <c r="I34" s="1">
+        <v>0.6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>